<commit_message>
Update execution substrates to disable 'ResolvesToAnAST' attribute across multiple files and enhance test results documentation. This commit modifies the 'ResolvesToAnAST' field to false in various JSON and TTL files, ensuring consistency in language candidate evaluations. Additionally, test results have been updated to reflect accurate execution durations across substrates, improving clarity and usability in reporting. Overall, these changes aim to streamline the evaluation framework and enhance documentation accuracy.
</commit_message>
<xml_diff>
--- a/execution-substratrates/xlsx/rulebook.xlsx
+++ b/execution-substratrates/xlsx/rulebook.xlsx
@@ -1398,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="2" t="b">
         <v>0</v>
@@ -1818,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Refactor language candidate evaluation criteria and enhance schema documentation
This commit updates the `README.SCHEMA.md` and `effortless-rulebook.json` files to refine the evaluation criteria for language candidates, including changes to the `HasGrammar` and `IsStableOntologyReference` fields, which are now marked as calculated. New formulas for `IsDescriptionOf` and adjustments to the `top_family_feud_answer` logic have been introduced to improve accuracy. Additionally, the `test-answers.json` and `test-results.md` files have been updated to reflect these changes, ensuring consistency across execution substrates. These enhancements aim to clarify the evaluation framework and improve the overall accuracy of language candidate assessments.
</commit_message>
<xml_diff>
--- a/execution-substratrates/xlsx/rulebook.xlsx
+++ b/execution-substratrates/xlsx/rulebook.xlsx
@@ -466,12 +466,12 @@
     <col width="27" customWidth="1" min="14" max="14"/>
     <col width="27" customWidth="1" min="15" max="15"/>
     <col width="22" customWidth="1" min="16" max="16"/>
-    <col width="28" customWidth="1" min="17" max="17"/>
-    <col width="13" customWidth="1" min="18" max="18"/>
-    <col width="15" customWidth="1" min="19" max="19"/>
-    <col width="29" customWidth="1" min="20" max="20"/>
-    <col width="21" customWidth="1" min="21" max="21"/>
-    <col width="17" customWidth="1" min="22" max="22"/>
+    <col width="13" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="17" customWidth="1" min="19" max="19"/>
+    <col width="21" customWidth="1" min="20" max="20"/>
+    <col width="29" customWidth="1" min="21" max="21"/>
+    <col width="28" customWidth="1" min="22" max="22"/>
     <col width="23" customWidth="1" min="23" max="23"/>
     <col width="26" customWidth="1" min="24" max="24"/>
     <col width="12" customWidth="1" min="25" max="25"/>
@@ -560,32 +560,32 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>IsOpenWorld</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>IsClosedWorld</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>IsDescriptionOf</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>DistanceFromConcept</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>IsOpenClosedWorldConflicted</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>DimensionalityWhileEditing</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>IsOpenWorld</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>IsClosedWorld</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>IsOpenClosedWorldConflicted</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>DistanceFromConcept</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>IsDescriptionOf</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
@@ -628,7 +628,7 @@
         <f>AND(
   $H2,
   $L2,
-  $V2,
+  $S2,
   $N2,
   $M2,
   $O2,
@@ -643,7 +643,7 @@
       <c r="G2" s="3">
         <f>IF(NOT($E2 = $F2),
   $B2 &amp; " " &amp; IF($E2, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F2, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T2, " - Open World vs. Closed World Conflict.")</f>
+  IF($F2, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U2, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H2" s="2" t="b">
@@ -674,30 +674,30 @@
       <c r="P2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="Q2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <f>$T2 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U2" s="3">
+        <f>AND($Q2, $R2)</f>
+        <v/>
+      </c>
+      <c r="V2" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" s="3">
-        <f>AND($R2, $S2)</f>
-        <v/>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V2" s="3">
-        <f>$U2 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W2" s="3">
-        <f>IF($U2 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T2 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X2" s="2" t="inlineStr">
@@ -733,7 +733,7 @@
         <f>AND(
   $H3,
   $L3,
-  $V3,
+  $S3,
   $N3,
   $M3,
   $O3,
@@ -748,7 +748,7 @@
       <c r="G3" s="3">
         <f>IF(NOT($E3 = $F3),
   $B3 &amp; " " &amp; IF($E3, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F3, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T3, " - Open World vs. Closed World Conflict.")</f>
+  IF($F3, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U3, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H3" s="2" t="b">
@@ -779,30 +779,30 @@
       <c r="P3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q3" s="2" t="inlineStr">
+      <c r="Q3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <f>$T3 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3">
+        <f>AND($Q3, $R3)</f>
+        <v/>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" s="3">
-        <f>AND($R3, $S3)</f>
-        <v/>
-      </c>
-      <c r="U3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" s="3">
-        <f>$U3 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W3" s="3">
-        <f>IF($U3 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T3 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X3" s="2" t="inlineStr">
@@ -838,7 +838,7 @@
         <f>AND(
   $H4,
   $L4,
-  $V4,
+  $S4,
   $N4,
   $M4,
   $O4,
@@ -853,7 +853,7 @@
       <c r="G4" s="3">
         <f>IF(NOT($E4 = $F4),
   $B4 &amp; " " &amp; IF($E4, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F4, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T4, " - Open World vs. Closed World Conflict.")</f>
+  IF($F4, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U4, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H4" s="2" t="b">
@@ -884,30 +884,30 @@
       <c r="P4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q4" s="2" t="inlineStr">
+      <c r="Q4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3">
+        <f>$T4 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U4" s="3">
+        <f>AND($Q4, $R4)</f>
+        <v/>
+      </c>
+      <c r="V4" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" s="3">
-        <f>AND($R4, $S4)</f>
-        <v/>
-      </c>
-      <c r="U4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V4" s="3">
-        <f>$U4 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W4" s="3">
-        <f>IF($U4 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T4 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X4" s="2" t="inlineStr">
@@ -943,7 +943,7 @@
         <f>AND(
   $H5,
   $L5,
-  $V5,
+  $S5,
   $N5,
   $M5,
   $O5,
@@ -958,7 +958,7 @@
       <c r="G5" s="3">
         <f>IF(NOT($E5 = $F5),
   $B5 &amp; " " &amp; IF($E5, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F5, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T5, " - Open World vs. Closed World Conflict.")</f>
+  IF($F5, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U5, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H5" s="2" t="b">
@@ -989,30 +989,30 @@
       <c r="P5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q5" s="2" t="inlineStr">
+      <c r="Q5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <f>$T5 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U5" s="3">
+        <f>AND($Q5, $R5)</f>
+        <v/>
+      </c>
+      <c r="V5" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" s="3">
-        <f>AND($R5, $S5)</f>
-        <v/>
-      </c>
-      <c r="U5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V5" s="3">
-        <f>$U5 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W5" s="3">
-        <f>IF($U5 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T5 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X5" s="2" t="inlineStr">
@@ -1048,7 +1048,7 @@
         <f>AND(
   $H6,
   $L6,
-  $V6,
+  $S6,
   $N6,
   $M6,
   $O6,
@@ -1063,7 +1063,7 @@
       <c r="G6" s="3">
         <f>IF(NOT($E6 = $F6),
   $B6 &amp; " " &amp; IF($E6, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F6, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T6, " - Open World vs. Closed World Conflict.")</f>
+  IF($F6, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U6, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H6" s="2" t="b">
@@ -1094,30 +1094,30 @@
       <c r="P6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="Q6" s="2" t="inlineStr">
+      <c r="Q6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3">
+        <f>$T6 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U6" s="3">
+        <f>AND($Q6, $R6)</f>
+        <v/>
+      </c>
+      <c r="V6" s="2" t="inlineStr">
         <is>
           <t>MultiDimensionalNonSymbolic</t>
         </is>
       </c>
-      <c r="R6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" s="3">
-        <f>AND($R6, $S6)</f>
-        <v/>
-      </c>
-      <c r="U6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V6" s="3">
-        <f>$U6 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W6" s="3">
-        <f>IF($U6 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T6 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X6" s="2" t="inlineStr">
@@ -1153,7 +1153,7 @@
         <f>AND(
   $H7,
   $L7,
-  $V7,
+  $S7,
   $N7,
   $M7,
   $O7,
@@ -1168,7 +1168,7 @@
       <c r="G7" s="3">
         <f>IF(NOT($E7 = $F7),
   $B7 &amp; " " &amp; IF($E7, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F7, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T7, " - Open World vs. Closed World Conflict.")</f>
+  IF($F7, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U7, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H7" s="2" t="b">
@@ -1199,30 +1199,30 @@
       <c r="P7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q7" s="2" t="inlineStr">
+      <c r="Q7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <f>$T7 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U7" s="3">
+        <f>AND($Q7, $R7)</f>
+        <v/>
+      </c>
+      <c r="V7" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" s="3">
-        <f>AND($R7, $S7)</f>
-        <v/>
-      </c>
-      <c r="U7" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V7" s="3">
-        <f>$U7 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W7" s="3">
-        <f>IF($U7 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T7 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X7" s="2" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <f>AND(
   $H8,
   $L8,
-  $V8,
+  $S8,
   $N8,
   $M8,
   $O8,
@@ -1273,7 +1273,7 @@
       <c r="G8" s="3">
         <f>IF(NOT($E8 = $F8),
   $B8 &amp; " " &amp; IF($E8, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F8, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T8, " - Open World vs. Closed World Conflict.")</f>
+  IF($F8, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U8, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H8" s="2" t="b">
@@ -1304,30 +1304,30 @@
       <c r="P8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q8" s="2" t="inlineStr">
+      <c r="Q8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" s="3">
+        <f>$T8 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
+        <f>AND($Q8, $R8)</f>
+        <v/>
+      </c>
+      <c r="V8" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" s="3">
-        <f>AND($R8, $S8)</f>
-        <v/>
-      </c>
-      <c r="U8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" s="3">
-        <f>$U8 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W8" s="3">
-        <f>IF($U8 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T8 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X8" s="2" t="inlineStr">
@@ -1363,7 +1363,7 @@
         <f>AND(
   $H9,
   $L9,
-  $V9,
+  $S9,
   $N9,
   $M9,
   $O9,
@@ -1378,7 +1378,7 @@
       <c r="G9" s="3">
         <f>IF(NOT($E9 = $F9),
   $B9 &amp; " " &amp; IF($E9, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F9, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T9, " - Open World vs. Closed World Conflict.")</f>
+  IF($F9, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U9, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H9" s="2" t="b">
@@ -1409,30 +1409,30 @@
       <c r="P9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q9" s="2" t="inlineStr">
+      <c r="Q9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" s="3">
+        <f>$T9 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" s="3">
+        <f>AND($Q9, $R9)</f>
+        <v/>
+      </c>
+      <c r="V9" s="2" t="inlineStr">
         <is>
           <t>MultiDimensionalNonSymbolic</t>
         </is>
       </c>
-      <c r="R9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9" s="3">
-        <f>AND($R9, $S9)</f>
-        <v/>
-      </c>
-      <c r="U9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V9" s="3">
-        <f>$U9 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W9" s="3">
-        <f>IF($U9 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T9 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X9" s="2" t="inlineStr">
@@ -1468,7 +1468,7 @@
         <f>AND(
   $H10,
   $L10,
-  $V10,
+  $S10,
   $N10,
   $M10,
   $O10,
@@ -1483,7 +1483,7 @@
       <c r="G10" s="3">
         <f>IF(NOT($E10 = $F10),
   $B10 &amp; " " &amp; IF($E10, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F10, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T10, " - Open World vs. Closed World Conflict.")</f>
+  IF($F10, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U10, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H10" s="2" t="b">
@@ -1514,30 +1514,30 @@
       <c r="P10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q10" s="2" t="inlineStr">
+      <c r="Q10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <f>$T10 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U10" s="3">
+        <f>AND($Q10, $R10)</f>
+        <v/>
+      </c>
+      <c r="V10" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T10" s="3">
-        <f>AND($R10, $S10)</f>
-        <v/>
-      </c>
-      <c r="U10" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V10" s="3">
-        <f>$U10 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W10" s="3">
-        <f>IF($U10 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T10 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X10" s="2" t="inlineStr">
@@ -1573,7 +1573,7 @@
         <f>AND(
   $H11,
   $L11,
-  $V11,
+  $S11,
   $N11,
   $M11,
   $O11,
@@ -1588,7 +1588,7 @@
       <c r="G11" s="3">
         <f>IF(NOT($E11 = $F11),
   $B11 &amp; " " &amp; IF($E11, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F11, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T11, " - Open World vs. Closed World Conflict.")</f>
+  IF($F11, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U11, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H11" s="2" t="b">
@@ -1619,30 +1619,30 @@
       <c r="P11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q11" s="2" t="inlineStr">
+      <c r="Q11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <f>$T11 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U11" s="3">
+        <f>AND($Q11, $R11)</f>
+        <v/>
+      </c>
+      <c r="V11" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" s="3">
-        <f>AND($R11, $S11)</f>
-        <v/>
-      </c>
-      <c r="U11" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V11" s="3">
-        <f>$U11 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W11" s="3">
-        <f>IF($U11 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T11 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X11" s="2" t="inlineStr">
@@ -1678,7 +1678,7 @@
         <f>AND(
   $H12,
   $L12,
-  $V12,
+  $S12,
   $N12,
   $M12,
   $O12,
@@ -1693,7 +1693,7 @@
       <c r="G12" s="3">
         <f>IF(NOT($E12 = $F12),
   $B12 &amp; " " &amp; IF($E12, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F12, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T12, " - Open World vs. Closed World Conflict.")</f>
+  IF($F12, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U12, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H12" s="2" t="b">
@@ -1724,30 +1724,30 @@
       <c r="P12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q12" s="2" t="inlineStr">
+      <c r="Q12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12" s="3">
+        <f>$T12 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
+        <f>AND($Q12, $R12)</f>
+        <v/>
+      </c>
+      <c r="V12" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" s="3">
-        <f>AND($R12, $S12)</f>
-        <v/>
-      </c>
-      <c r="U12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" s="3">
-        <f>$U12 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W12" s="3">
-        <f>IF($U12 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T12 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X12" s="2" t="inlineStr">
@@ -1783,7 +1783,7 @@
         <f>AND(
   $H13,
   $L13,
-  $V13,
+  $S13,
   $N13,
   $M13,
   $O13,
@@ -1798,7 +1798,7 @@
       <c r="G13" s="3">
         <f>IF(NOT($E13 = $F13),
   $B13 &amp; " " &amp; IF($E13, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F13, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T13, " - Open World vs. Closed World Conflict.")</f>
+  IF($F13, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U13, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H13" s="2" t="b">
@@ -1829,30 +1829,30 @@
       <c r="P13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="Q13" s="2" t="inlineStr">
+      <c r="Q13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" s="3">
+        <f>$T13 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" s="3">
+        <f>AND($Q13, $R13)</f>
+        <v/>
+      </c>
+      <c r="V13" s="2" t="inlineStr">
         <is>
           <t>MultiDimensionalNonSymbolic</t>
         </is>
       </c>
-      <c r="R13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" s="3">
-        <f>AND($R13, $S13)</f>
-        <v/>
-      </c>
-      <c r="U13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V13" s="3">
-        <f>$U13 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W13" s="3">
-        <f>IF($U13 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T13 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X13" s="2" t="inlineStr">
@@ -1888,7 +1888,7 @@
         <f>AND(
   $H14,
   $L14,
-  $V14,
+  $S14,
   $N14,
   $M14,
   $O14,
@@ -1903,7 +1903,7 @@
       <c r="G14" s="3">
         <f>IF(NOT($E14 = $F14),
   $B14 &amp; " " &amp; IF($E14, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F14, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T14, " - Open World vs. Closed World Conflict.")</f>
+  IF($F14, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U14, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H14" s="2" t="b">
@@ -1934,30 +1934,30 @@
       <c r="P14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q14" s="2" t="inlineStr">
+      <c r="Q14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3">
+        <f>$T14 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U14" s="3">
+        <f>AND($Q14, $R14)</f>
+        <v/>
+      </c>
+      <c r="V14" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T14" s="3">
-        <f>AND($R14, $S14)</f>
-        <v/>
-      </c>
-      <c r="U14" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V14" s="3">
-        <f>$U14 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W14" s="3">
-        <f>IF($U14 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T14 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X14" s="2" t="inlineStr">
@@ -1993,7 +1993,7 @@
         <f>AND(
   $H15,
   $L15,
-  $V15,
+  $S15,
   $N15,
   $M15,
   $O15,
@@ -2008,7 +2008,7 @@
       <c r="G15" s="3">
         <f>IF(NOT($E15 = $F15),
   $B15 &amp; " " &amp; IF($E15, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F15, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T15, " - Open World vs. Closed World Conflict.")</f>
+  IF($F15, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U15, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H15" s="2" t="b">
@@ -2039,30 +2039,30 @@
       <c r="P15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="Q15" s="2" t="inlineStr">
+      <c r="Q15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
+        <f>$T15 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U15" s="3">
+        <f>AND($Q15, $R15)</f>
+        <v/>
+      </c>
+      <c r="V15" s="2" t="inlineStr">
         <is>
           <t>MultiDimensionalNonSymbolic</t>
         </is>
       </c>
-      <c r="R15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T15" s="3">
-        <f>AND($R15, $S15)</f>
-        <v/>
-      </c>
-      <c r="U15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V15" s="3">
-        <f>$U15 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W15" s="3">
-        <f>IF($U15 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T15 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X15" s="2" t="inlineStr">
@@ -2098,7 +2098,7 @@
         <f>AND(
   $H16,
   $L16,
-  $V16,
+  $S16,
   $N16,
   $M16,
   $O16,
@@ -2113,7 +2113,7 @@
       <c r="G16" s="3">
         <f>IF(NOT($E16 = $F16),
   $B16 &amp; " " &amp; IF($E16, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F16, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T16, " - Open World vs. Closed World Conflict.")</f>
+  IF($F16, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U16, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H16" s="2" t="b">
@@ -2144,30 +2144,30 @@
       <c r="P16" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q16" s="2" t="inlineStr">
+      <c r="Q16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
+        <f>$T16 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U16" s="3">
+        <f>AND($Q16, $R16)</f>
+        <v/>
+      </c>
+      <c r="V16" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16" s="3">
-        <f>AND($R16, $S16)</f>
-        <v/>
-      </c>
-      <c r="U16" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V16" s="3">
-        <f>$U16 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W16" s="3">
-        <f>IF($U16 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T16 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X16" s="2" t="inlineStr">
@@ -2203,7 +2203,7 @@
         <f>AND(
   $H17,
   $L17,
-  $V17,
+  $S17,
   $N17,
   $M17,
   $O17,
@@ -2218,7 +2218,7 @@
       <c r="G17" s="3">
         <f>IF(NOT($E17 = $F17),
   $B17 &amp; " " &amp; IF($E17, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F17, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T17, " - Open World vs. Closed World Conflict.")</f>
+  IF($F17, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U17, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H17" s="2" t="b">
@@ -2249,30 +2249,30 @@
       <c r="P17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="Q17" s="2" t="inlineStr">
+      <c r="Q17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <f>$T17 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
+        <f>AND($Q17, $R17)</f>
+        <v/>
+      </c>
+      <c r="V17" s="2" t="inlineStr">
         <is>
           <t>MultiDimensionalNonSymbolic</t>
         </is>
       </c>
-      <c r="R17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T17" s="3">
-        <f>AND($R17, $S17)</f>
-        <v/>
-      </c>
-      <c r="U17" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V17" s="3">
-        <f>$U17 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W17" s="3">
-        <f>IF($U17 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T17 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X17" s="2" t="inlineStr">
@@ -2308,7 +2308,7 @@
         <f>AND(
   $H18,
   $L18,
-  $V18,
+  $S18,
   $N18,
   $M18,
   $O18,
@@ -2323,7 +2323,7 @@
       <c r="G18" s="3">
         <f>IF(NOT($E18 = $F18),
   $B18 &amp; " " &amp; IF($E18, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F18, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T18, " - Open World vs. Closed World Conflict.")</f>
+  IF($F18, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U18, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H18" s="2" t="b">
@@ -2354,30 +2354,30 @@
       <c r="P18" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q18" s="2" t="inlineStr">
+      <c r="Q18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <f>$T18 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U18" s="3">
+        <f>AND($Q18, $R18)</f>
+        <v/>
+      </c>
+      <c r="V18" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18" s="3">
-        <f>AND($R18, $S18)</f>
-        <v/>
-      </c>
-      <c r="U18" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V18" s="3">
-        <f>$U18 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W18" s="3">
-        <f>IF($U18 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T18 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X18" s="2" t="inlineStr">
@@ -2413,7 +2413,7 @@
         <f>AND(
   $H19,
   $L19,
-  $V19,
+  $S19,
   $N19,
   $M19,
   $O19,
@@ -2428,7 +2428,7 @@
       <c r="G19" s="3">
         <f>IF(NOT($E19 = $F19),
   $B19 &amp; " " &amp; IF($E19, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F19, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T19, " - Open World vs. Closed World Conflict.")</f>
+  IF($F19, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U19, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H19" s="2" t="b">
@@ -2459,30 +2459,30 @@
       <c r="P19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q19" s="2" t="inlineStr">
+      <c r="Q19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S19" s="3">
+        <f>$T19 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U19" s="3">
+        <f>AND($Q19, $R19)</f>
+        <v/>
+      </c>
+      <c r="V19" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T19" s="3">
-        <f>AND($R19, $S19)</f>
-        <v/>
-      </c>
-      <c r="U19" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V19" s="3">
-        <f>$U19 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W19" s="3">
-        <f>IF($U19 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T19 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X19" s="2" t="inlineStr">
@@ -2518,7 +2518,7 @@
         <f>AND(
   $H20,
   $L20,
-  $V20,
+  $S20,
   $N20,
   $M20,
   $O20,
@@ -2533,7 +2533,7 @@
       <c r="G20" s="3">
         <f>IF(NOT($E20 = $F20),
   $B20 &amp; " " &amp; IF($E20, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F20, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T20, " - Open World vs. Closed World Conflict.")</f>
+  IF($F20, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U20, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H20" s="2" t="b">
@@ -2564,30 +2564,30 @@
       <c r="P20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q20" s="2" t="inlineStr">
+      <c r="Q20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <f>$T20 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3">
+        <f>AND($Q20, $R20)</f>
+        <v/>
+      </c>
+      <c r="V20" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T20" s="3">
-        <f>AND($R20, $S20)</f>
-        <v/>
-      </c>
-      <c r="U20" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V20" s="3">
-        <f>$U20 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W20" s="3">
-        <f>IF($U20 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T20 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X20" s="2" t="inlineStr">
@@ -2623,7 +2623,7 @@
         <f>AND(
   $H21,
   $L21,
-  $V21,
+  $S21,
   $N21,
   $M21,
   $O21,
@@ -2638,7 +2638,7 @@
       <c r="G21" s="3">
         <f>IF(NOT($E21 = $F21),
   $B21 &amp; " " &amp; IF($E21, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F21, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T21, " - Open World vs. Closed World Conflict.")</f>
+  IF($F21, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U21, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H21" s="2" t="b">
@@ -2669,30 +2669,30 @@
       <c r="P21" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q21" s="2" t="inlineStr">
+      <c r="Q21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <f>$T21 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U21" s="3">
+        <f>AND($Q21, $R21)</f>
+        <v/>
+      </c>
+      <c r="V21" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T21" s="3">
-        <f>AND($R21, $S21)</f>
-        <v/>
-      </c>
-      <c r="U21" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V21" s="3">
-        <f>$U21 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W21" s="3">
-        <f>IF($U21 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T21 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X21" s="2" t="inlineStr">
@@ -2728,7 +2728,7 @@
         <f>AND(
   $H22,
   $L22,
-  $V22,
+  $S22,
   $N22,
   $M22,
   $O22,
@@ -2743,7 +2743,7 @@
       <c r="G22" s="3">
         <f>IF(NOT($E22 = $F22),
   $B22 &amp; " " &amp; IF($E22, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F22, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T22, " - Open World vs. Closed World Conflict.")</f>
+  IF($F22, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U22, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H22" s="2" t="b">
@@ -2774,30 +2774,30 @@
       <c r="P22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q22" s="2" t="inlineStr">
+      <c r="Q22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <f>$T22 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U22" s="3">
+        <f>AND($Q22, $R22)</f>
+        <v/>
+      </c>
+      <c r="V22" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R22" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T22" s="3">
-        <f>AND($R22, $S22)</f>
-        <v/>
-      </c>
-      <c r="U22" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V22" s="3">
-        <f>$U22 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W22" s="3">
-        <f>IF($U22 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T22 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X22" s="2" t="inlineStr">
@@ -2833,7 +2833,7 @@
         <f>AND(
   $H23,
   $L23,
-  $V23,
+  $S23,
   $N23,
   $M23,
   $O23,
@@ -2848,7 +2848,7 @@
       <c r="G23" s="3">
         <f>IF(NOT($E23 = $F23),
   $B23 &amp; " " &amp; IF($E23, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F23, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T23, " - Open World vs. Closed World Conflict.")</f>
+  IF($F23, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U23, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H23" s="2" t="b">
@@ -2879,30 +2879,30 @@
       <c r="P23" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q23" s="2" t="inlineStr">
+      <c r="Q23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3">
+        <f>$T23 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U23" s="3">
+        <f>AND($Q23, $R23)</f>
+        <v/>
+      </c>
+      <c r="V23" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T23" s="3">
-        <f>AND($R23, $S23)</f>
-        <v/>
-      </c>
-      <c r="U23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V23" s="3">
-        <f>$U23 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W23" s="3">
-        <f>IF($U23 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T23 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X23" s="2" t="inlineStr">
@@ -2938,7 +2938,7 @@
         <f>AND(
   $H24,
   $L24,
-  $V24,
+  $S24,
   $N24,
   $M24,
   $O24,
@@ -2953,7 +2953,7 @@
       <c r="G24" s="3">
         <f>IF(NOT($E24 = $F24),
   $B24 &amp; " " &amp; IF($E24, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F24, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T24, " - Open World vs. Closed World Conflict.")</f>
+  IF($F24, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U24, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H24" s="2" t="b">
@@ -2984,30 +2984,30 @@
       <c r="P24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q24" s="2" t="inlineStr">
+      <c r="Q24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S24" s="3">
+        <f>$T24 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3">
+        <f>AND($Q24, $R24)</f>
+        <v/>
+      </c>
+      <c r="V24" s="2" t="inlineStr">
         <is>
           <t>MultiDimensionalNonSymbolic</t>
         </is>
       </c>
-      <c r="R24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T24" s="3">
-        <f>AND($R24, $S24)</f>
-        <v/>
-      </c>
-      <c r="U24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="V24" s="3">
-        <f>$U24 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W24" s="3">
-        <f>IF($U24 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T24 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X24" s="2" t="inlineStr">
@@ -3043,7 +3043,7 @@
         <f>AND(
   $H25,
   $L25,
-  $V25,
+  $S25,
   $N25,
   $M25,
   $O25,
@@ -3058,7 +3058,7 @@
       <c r="G25" s="3">
         <f>IF(NOT($E25 = $F25),
   $B25 &amp; " " &amp; IF($E25, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F25, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T25, " - Open World vs. Closed World Conflict.")</f>
+  IF($F25, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U25, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H25" s="2" t="b">
@@ -3089,30 +3089,30 @@
       <c r="P25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q25" s="2" t="inlineStr">
+      <c r="Q25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S25" s="3">
+        <f>$T25 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U25" s="3">
+        <f>AND($Q25, $R25)</f>
+        <v/>
+      </c>
+      <c r="V25" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R25" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S25" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T25" s="3">
-        <f>AND($R25, $S25)</f>
-        <v/>
-      </c>
-      <c r="U25" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V25" s="3">
-        <f>$U25 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W25" s="3">
-        <f>IF($U25 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T25 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X25" s="2" t="inlineStr">
@@ -3148,7 +3148,7 @@
         <f>AND(
   $H26,
   $L26,
-  $V26,
+  $S26,
   $N26,
   $M26,
   $O26,
@@ -3163,7 +3163,7 @@
       <c r="G26" s="3">
         <f>IF(NOT($E26 = $F26),
   $B26 &amp; " " &amp; IF($E26, "Is", "Isn't") &amp; " a Family Feud Language, but " &amp; 
-  IF($F26, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($T26, " - Open World vs. Closed World Conflict.")</f>
+  IF($F26, "Is", "Is Not") &amp; " marked as a 'Language Candidate.'") &amp; IF($U26, " - Open World vs. Closed World Conflict.")</f>
         <v/>
       </c>
       <c r="H26" s="2" t="b">
@@ -3194,30 +3194,30 @@
       <c r="P26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="Q26" s="2" t="inlineStr">
+      <c r="Q26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S26" s="3">
+        <f>$T26 &gt; 1</f>
+        <v/>
+      </c>
+      <c r="T26" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U26" s="3">
+        <f>AND($Q26, $R26)</f>
+        <v/>
+      </c>
+      <c r="V26" s="2" t="inlineStr">
         <is>
           <t>OneDimensionalSymbolic</t>
         </is>
       </c>
-      <c r="R26" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S26" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T26" s="3">
-        <f>AND($R26, $S26)</f>
-        <v/>
-      </c>
-      <c r="U26" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V26" s="3">
-        <f>$U26 &gt; 1</f>
-        <v/>
-      </c>
       <c r="W26" s="3">
-        <f>IF($U26 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
+        <f>IF($T26 = 1, "IsMirrorOf", "IsDescriptionOf")</f>
         <v/>
       </c>
       <c r="X26" s="2" t="inlineStr">

</xml_diff>